<commit_message>
(v2.1.1.9225) fix geom_hline()/_vline() in MIC plotting, add EUCAT 1.2 in full, add London contribs, fix mo codes, add Kleb pneu complex
</commit_message>
<xml_diff>
--- a/data-raw/microorganisms.groups.xlsx
+++ b/data-raw/microorganisms.groups.xlsx
@@ -369,22 +369,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:D522"/>
+  <dimension ref="A1:D535"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
+      <c r="A1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B1" t="e">
+        <v>#N/A</v>
       </c>
       <c r="C1" t="inlineStr">
         <is>
@@ -7264,924 +7260,924 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>F_CANDD_FRMN</t>
+          <t>B_KLBSL_AFRC</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Candida fermentati</t>
+          <t>Klebsiella africana</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>F_MYRZY_CRBB</t>
+          <t>B_KLBSL_PNMN</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Meyerozyma caribbica</t>
+          <t>Klebsiella pneumoniae</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>F_MYRZY_CRPP</t>
+          <t>B_KLBSL_PNMN_OZAN</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Meyerozyma carpophila</t>
+          <t>Klebsiella pneumoniae ozaenae</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR</t>
+          <t>B_KLBSL_PNMN_PNMN</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii</t>
+          <t>Klebsiella pneumoniae pneumoniae</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>F_MYRZY_CRPP</t>
+          <t>B_KLBSL_PNMN_RHNS</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii carpophila</t>
+          <t>Klebsiella pneumoniae rhinoscleromatis</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR</t>
+          <t>B_KLBSL_QSPN</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii japonica</t>
+          <t>Klebsiella quasipneumoniae</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR</t>
+          <t>B_KLBSL_QSPN_QSPN</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii muhira</t>
+          <t>Klebsiella quasipneumoniae quasipneumoniae</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>F_MYRZY_GLLR</t>
+          <t>B_KLBSL_QSPN_SMLP</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Meyerozyma guilliermondii pseudoguilliermondii</t>
+          <t>Klebsiella quasipneumoniae similipneumoniae</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM</t>
+          <t>B_KLBSL_QSVR</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>Mycobacterium avium-intracellulare complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Mycobacterium avium</t>
+          <t>Klebsiella quasivariicola</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM_AVIM</t>
+          <t>B_KLBSL_VRCL</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>Mycobacterium avium-intracellulare complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Mycobacterium avium avium</t>
+          <t>Klebsiella variicola</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM_PRTB</t>
+          <t>B_KLBSL_VRCL_TRPC</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>Mycobacterium avium-intracellulare complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Mycobacterium avium paratuberculosis</t>
+          <t>Klebsiella variicola tropica</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM_SLVT</t>
+          <t>B_KLBSL_VRCL_LNSS</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>Mycobacterium avium-intracellulare complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Mycobacterium avium silvaticum</t>
+          <t>Klebsiella variicola tropicalensis</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM-C</t>
+          <t>B_KLBSL_PNMN-C</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>B_MYCBC_LLRE</t>
+          <t>B_KLBSL_VRCL_VRCL</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>Mycobacterium avium-intracellulare complex</t>
+          <t>Klebsiella pneumoniae complex</t>
         </is>
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Mycobacterium intracellulare</t>
+          <t>Klebsiella variicola variicola</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM-C</t>
+          <t>F_MYRZY_GLLR-C</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>B_MYCBC_LLRE_CHMR</t>
+          <t>F_CANDD_FRMN</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>Mycobacterium avium-intracellulare complex</t>
+          <t>Meyerozyma guilliermondii complex</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Mycobacterium intracellulare chimaera</t>
+          <t>Candida fermentati</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM-C</t>
+          <t>F_MYRZY_GLLR-C</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>B_MYCBC_LLRE_INTR</t>
+          <t>F_MYRZY_CRBB</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>Mycobacterium avium-intracellulare complex</t>
+          <t>Meyerozyma guilliermondii complex</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Mycobacterium intracellulare intracellulare</t>
+          <t>Meyerozyma caribbica</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>B_MYCBC_AVIM-C</t>
+          <t>F_MYRZY_GLLR-C</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>B_MYCBC_LLRE_CHMR</t>
+          <t>F_MYRZY_CRPP</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>Mycobacterium avium-intracellulare complex</t>
+          <t>Meyerozyma guilliermondii complex</t>
         </is>
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Mycobacterium intracellulare yongonense</t>
+          <t>Meyerozyma carpophila</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>F_MYRZY_GLLR-C</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>F_MYRZY_GLLR</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Meyerozyma guilliermondii complex</t>
         </is>
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Mycobacterium africanum</t>
+          <t>Meyerozyma guilliermondii</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>F_MYRZY_GLLR-C</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>F_MYRZY_CRPP</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Meyerozyma guilliermondii complex</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Mycobacterium bovis</t>
+          <t>Meyerozyma guilliermondii carpophila</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>F_MYRZY_GLLR-C</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>F_MYRZY_GLLR</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Meyerozyma guilliermondii complex</t>
         </is>
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Mycobacterium bovis bovis</t>
+          <t>Meyerozyma guilliermondii japonica</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>F_MYRZY_GLLR-C</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>F_MYRZY_GLLR</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Meyerozyma guilliermondii complex</t>
         </is>
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Mycobacterium bovis caprae</t>
+          <t>Meyerozyma guilliermondii muhira</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>F_MYRZY_GLLR-C</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>F_MYRZY_GLLR</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Meyerozyma guilliermondii complex</t>
         </is>
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>Mycobacterium caprae</t>
+          <t>Meyerozyma guilliermondii pseudoguilliermondii</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>B_MYCBC_AVIM-C</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>B_MYCBC_AVIM</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Mycobacterium avium-intracellulare complex</t>
         </is>
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>Mycobacterium microti</t>
+          <t>Mycobacterium avium</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>B_MYCBC_AVIM-C</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>B_MYCBC_MUNG</t>
+          <t>B_MYCBC_AVIM_AVIM</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Mycobacterium avium-intracellulare complex</t>
         </is>
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>Mycobacterium mungi</t>
+          <t>Mycobacterium avium avium</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>B_MYCBC_AVIM-C</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>B_MYCBC_ORYG</t>
+          <t>B_MYCBC_AVIM_PRTB</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Mycobacterium avium-intracellulare complex</t>
         </is>
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>Mycobacterium orygis</t>
+          <t>Mycobacterium avium paratuberculosis</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>B_MYCBC_AVIM-C</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>B_MYCBC_AVIM_SLVT</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Mycobacterium avium-intracellulare complex</t>
         </is>
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Mycobacterium pinnipedii</t>
+          <t>Mycobacterium avium silvaticum</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>B_MYCBC_AVIM-C</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>B_MYCBC_LLRE</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Mycobacterium avium-intracellulare complex</t>
         </is>
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis</t>
+          <t>Mycobacterium intracellulare</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>B_MYCBC_AVIM-C</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>B_MYCBC_LLRE_CHMR</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Mycobacterium avium-intracellulare complex</t>
         </is>
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis caprae</t>
+          <t>Mycobacterium intracellulare chimaera</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC-C</t>
+          <t>B_MYCBC_AVIM-C</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>B_MYCBC_TBRC</t>
+          <t>B_MYCBC_LLRE_INTR</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis complex</t>
+          <t>Mycobacterium avium-intracellulare complex</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>Mycobacterium tuberculosis tuberculosis</t>
+          <t>Mycobacterium intracellulare intracellulare</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>B_PSDMN_FLRS-C</t>
+          <t>B_MYCBC_AVIM-C</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>B_PSDMN_FLRS</t>
+          <t>B_MYCBC_LLRE_CHMR</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>Pseudomonas fluorescens complex</t>
+          <t>Mycobacterium avium-intracellulare complex</t>
         </is>
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Pseudomonas fluorescens</t>
+          <t>Mycobacterium intracellulare yongonense</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>B_MYCBC_ABSC_ABSC</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>Mycobacterium abscessus abscessus</t>
+          <t>Mycobacterium africanum</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>B_MYCBC_ABSC_BLLT</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>Mycobacterium abscessus bolletii</t>
+          <t>Mycobacterium bovis</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>B_MYCBC_ABSC_MSSL</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>Mycobacterium abscessus massiliense</t>
+          <t>Mycobacterium bovis bovis</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>B_MYCBC_AGRI</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>Mycobacterium agri</t>
+          <t>Mycobacterium bovis caprae</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>B_MYCBC_ACHN</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>Mycobacterium aichiense</t>
+          <t>Mycobacterium caprae</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>B_MYCBC_ALGR</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>Mycobacterium algericum</t>
+          <t>Mycobacterium microti</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>B_MYCBC_ALVE</t>
+          <t>B_MYCBC_MUNG</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>Mycobacterium alvei</t>
+          <t>Mycobacterium mungi</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>B_MYCBC_ANYN</t>
+          <t>B_MYCBC_ORYG</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>Mycobacterium anyangense</t>
+          <t>Mycobacterium orygis</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>B_MYCBC_ARBN</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>Mycobacterium arabiense</t>
+          <t>Mycobacterium pinnipedii</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>B_MYCBC_ARMT</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>Mycobacterium aromaticivorans</t>
+          <t>Mycobacterium tuberculosis</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>B_MYCBC_ABGN</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>Mycobacterium aubagnense</t>
+          <t>Mycobacterium tuberculosis caprae</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_MYCBC_TBRC-C</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>B_MYCBC_AURM</t>
+          <t>B_MYCBC_TBRC</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Mycobacterium tuberculosis complex</t>
         </is>
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>Mycobacterium aurum</t>
+          <t>Mycobacterium tuberculosis tuberculosis</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>B_MYCBC_RGM</t>
+          <t>B_PSDMN_FLRS-C</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>B_MYCBC_ASTR</t>
+          <t>B_PSDMN_FLRS</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>Rapidly growing Mycobacterium (RGM)</t>
+          <t>Pseudomonas fluorescens complex</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>Mycobacterium austroafricanum</t>
+          <t>Pseudomonas fluorescens</t>
         </is>
       </c>
     </row>
@@ -8193,7 +8189,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>B_MYCBC_BCTR</t>
+          <t>B_MYCBC_ABSC_ABSC</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
@@ -8203,7 +8199,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>Mycobacterium bacteremicum</t>
+          <t>Mycobacterium abscessus abscessus</t>
         </is>
       </c>
     </row>
@@ -8215,7 +8211,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>B_MYCBC_BNCK</t>
+          <t>B_MYCBC_ABSC_BLLT</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
@@ -8225,7 +8221,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>Mycobacterium boenickei</t>
+          <t>Mycobacterium abscessus bolletii</t>
         </is>
       </c>
     </row>
@@ -8237,7 +8233,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>B_MYCBC_BRGL</t>
+          <t>B_MYCBC_ABSC_MSSL</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
@@ -8247,7 +8243,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>Mycobacterium bourgelatii</t>
+          <t>Mycobacterium abscessus massiliense</t>
         </is>
       </c>
     </row>
@@ -8259,7 +8255,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>B_MYCBC_BRSB</t>
+          <t>B_MYCBC_AGRI</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
@@ -8269,7 +8265,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>Mycobacterium brisbanense</t>
+          <t>Mycobacterium agri</t>
         </is>
       </c>
     </row>
@@ -8281,7 +8277,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>B_MYCBC_BRUM</t>
+          <t>B_MYCBC_ACHN</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
@@ -8291,7 +8287,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>Mycobacterium brumae</t>
+          <t>Mycobacterium aichiense</t>
         </is>
       </c>
     </row>
@@ -8303,7 +8299,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>B_MYCBC_CNRS</t>
+          <t>B_MYCBC_ALGR</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
@@ -8313,7 +8309,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>Mycobacterium canariasense</t>
+          <t>Mycobacterium algericum</t>
         </is>
       </c>
     </row>
@@ -8325,7 +8321,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>B_MYCBC_CLRF</t>
+          <t>B_MYCBC_ALVE</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
@@ -8335,7 +8331,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>Mycobacterium celeriflavum</t>
+          <t>Mycobacterium alvei</t>
         </is>
       </c>
     </row>
@@ -8347,7 +8343,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>B_MYCBC_CHLN</t>
+          <t>B_MYCBC_ANYN</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
@@ -8357,7 +8353,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>Mycobacterium chelonae</t>
+          <t>Mycobacterium anyangense</t>
         </is>
       </c>
     </row>
@@ -8369,7 +8365,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>B_MYCBC_ABSC</t>
+          <t>B_MYCBC_ARBN</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
@@ -8379,7 +8375,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>Mycobacterium chelonae abscessus</t>
+          <t>Mycobacterium arabiense</t>
         </is>
       </c>
     </row>
@@ -8391,7 +8387,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>B_MYCBC_CHLN_BVST</t>
+          <t>B_MYCBC_ARMT</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
@@ -8401,7 +8397,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>Mycobacterium chelonae bovis</t>
+          <t>Mycobacterium aromaticivorans</t>
         </is>
       </c>
     </row>
@@ -8413,7 +8409,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>B_MYCBC_CHLN_CHLN</t>
+          <t>B_MYCBC_ABGN</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
@@ -8423,7 +8419,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>Mycobacterium chelonae chelonae</t>
+          <t>Mycobacterium aubagnense</t>
         </is>
       </c>
     </row>
@@ -8435,7 +8431,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>B_MYCBC_CHLN_GWNK</t>
+          <t>B_MYCBC_AURM</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
@@ -8445,7 +8441,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>Mycobacterium chelonae gwanakae</t>
+          <t>Mycobacterium aurum</t>
         </is>
       </c>
     </row>
@@ -8457,7 +8453,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>B_MYCBC_CHIT</t>
+          <t>B_MYCBC_ASTR</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
@@ -8467,7 +8463,7 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>Mycobacterium chitae</t>
+          <t>Mycobacterium austroafricanum</t>
         </is>
       </c>
     </row>
@@ -8479,7 +8475,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>B_MYCBC_CHLR</t>
+          <t>B_MYCBC_BCTR</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
@@ -8489,7 +8485,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>Mycobacterium chlorophenolicum</t>
+          <t>Mycobacterium bacteremicum</t>
         </is>
       </c>
     </row>
@@ -8501,7 +8497,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>B_MYCBC_CHBN</t>
+          <t>B_MYCBC_BNCK</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
@@ -8511,7 +8507,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Mycobacterium chubuense</t>
+          <t>Mycobacterium boenickei</t>
         </is>
       </c>
     </row>
@@ -8523,7 +8519,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>B_MYCBC_CNFL</t>
+          <t>B_MYCBC_BRGL</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
@@ -8533,7 +8529,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>Mycobacterium confluentis</t>
+          <t>Mycobacterium bourgelatii</t>
         </is>
       </c>
     </row>
@@ -8545,7 +8541,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>B_MYCBC_CSMT</t>
+          <t>B_MYCBC_BRSB</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
@@ -8555,7 +8551,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>Mycobacterium cosmeticum</t>
+          <t>Mycobacterium brisbanense</t>
         </is>
       </c>
     </row>
@@ -8567,7 +8563,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>B_MYCBC_CRCN</t>
+          <t>B_MYCBC_BRUM</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
@@ -8577,7 +8573,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>Mycobacterium crocinum</t>
+          <t>Mycobacterium brumae</t>
         </is>
       </c>
     </row>
@@ -8589,7 +8585,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>B_MYCBC_DRNH</t>
+          <t>B_MYCBC_CNRS</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
@@ -8599,7 +8595,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>Mycobacterium diernhoferi</t>
+          <t>Mycobacterium canariasense</t>
         </is>
       </c>
     </row>
@@ -8611,7 +8607,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>B_MYCBC_DUVL</t>
+          <t>B_MYCBC_CLRF</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
@@ -8621,7 +8617,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>Mycobacterium duvalii</t>
+          <t>Mycobacterium celeriflavum</t>
         </is>
       </c>
     </row>
@@ -8633,7 +8629,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>B_MYCBC_ELPH</t>
+          <t>B_MYCBC_CHLN</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
@@ -8643,7 +8639,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>Mycobacterium elephantis</t>
+          <t>Mycobacterium chelonae</t>
         </is>
       </c>
     </row>
@@ -8655,7 +8651,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>B_MYCBC_FLLX</t>
+          <t>B_MYCBC_ABSC</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
@@ -8665,7 +8661,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>Mycobacterium fallax</t>
+          <t>Mycobacterium chelonae abscessus</t>
         </is>
       </c>
     </row>
@@ -8677,7 +8673,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>B_MYCBC_FLVS</t>
+          <t>B_MYCBC_CHLN_BVST</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
@@ -8687,7 +8683,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>Mycobacterium flavescens</t>
+          <t>Mycobacterium chelonae bovis</t>
         </is>
       </c>
     </row>
@@ -8699,7 +8695,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>B_MYCBC_VRNS</t>
+          <t>B_MYCBC_CHLN_CHLN</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -8709,7 +8705,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>Mycobacterium fluoranthenivorans</t>
+          <t>Mycobacterium chelonae chelonae</t>
         </is>
       </c>
     </row>
@@ -8721,7 +8717,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>B_MYCBC_FRTT</t>
+          <t>B_MYCBC_CHLN_GWNK</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
@@ -8731,7 +8727,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>Mycobacterium fortuitum</t>
+          <t>Mycobacterium chelonae gwanakae</t>
         </is>
       </c>
     </row>
@@ -8743,7 +8739,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>B_MYCBC_FRTT_ACTM</t>
+          <t>B_MYCBC_CHIT</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
@@ -8753,7 +8749,7 @@
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>Mycobacterium fortuitum acetamidolyticum</t>
+          <t>Mycobacterium chitae</t>
         </is>
       </c>
     </row>
@@ -8765,7 +8761,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>B_MYCBC_FRTT_FRTT</t>
+          <t>B_MYCBC_CHLR</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
@@ -8775,7 +8771,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>Mycobacterium fortuitum fortuitum</t>
+          <t>Mycobacterium chlorophenolicum</t>
         </is>
       </c>
     </row>
@@ -8787,7 +8783,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>B_MYCBC_FRNK</t>
+          <t>B_MYCBC_CHBN</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
@@ -8797,7 +8793,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>Mycobacterium franklinii</t>
+          <t>Mycobacterium chubuense</t>
         </is>
       </c>
     </row>
@@ -8809,7 +8805,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>B_MYCBC_FRDR</t>
+          <t>B_MYCBC_CNFL</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
@@ -8819,7 +8815,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>Mycobacterium frederiksbergense</t>
+          <t>Mycobacterium confluentis</t>
         </is>
       </c>
     </row>
@@ -8831,7 +8827,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>B_MYCBC_GADM</t>
+          <t>B_MYCBC_CSMT</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
@@ -8841,7 +8837,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>Mycobacterium gadium</t>
+          <t>Mycobacterium cosmeticum</t>
         </is>
       </c>
     </row>
@@ -8853,7 +8849,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>B_MYCBC_GLVM</t>
+          <t>B_MYCBC_CRCN</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
@@ -8863,7 +8859,7 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>Mycobacterium gilvum</t>
+          <t>Mycobacterium crocinum</t>
         </is>
       </c>
     </row>
@@ -8875,7 +8871,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>B_MYCBC_GOOD</t>
+          <t>B_MYCBC_DRNH</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
@@ -8885,7 +8881,7 @@
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>Mycobacterium goodii</t>
+          <t>Mycobacterium diernhoferi</t>
         </is>
       </c>
     </row>
@@ -8897,7 +8893,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>B_MYCBC_HSSC</t>
+          <t>B_MYCBC_DUVL</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
@@ -8907,7 +8903,7 @@
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>Mycobacterium hassiacum</t>
+          <t>Mycobacterium duvalii</t>
         </is>
       </c>
     </row>
@@ -8919,7 +8915,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>B_MYCBC_HPPC</t>
+          <t>B_MYCBC_ELPH</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
@@ -8929,7 +8925,7 @@
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>Mycobacterium hippocampi</t>
+          <t>Mycobacterium elephantis</t>
         </is>
       </c>
     </row>
@@ -8941,7 +8937,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>B_MYCBC_HDLR</t>
+          <t>B_MYCBC_FLLX</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
@@ -8951,7 +8947,7 @@
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>Mycobacterium hodleri</t>
+          <t>Mycobacterium fallax</t>
         </is>
       </c>
     </row>
@@ -8963,7 +8959,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>B_MYCBC_HLST</t>
+          <t>B_MYCBC_FLVS</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
@@ -8973,7 +8969,7 @@
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>Mycobacterium holsaticum</t>
+          <t>Mycobacterium flavescens</t>
         </is>
       </c>
     </row>
@@ -8985,7 +8981,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>B_MYCBC_HSTN</t>
+          <t>B_MYCBC_VRNS</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
@@ -8995,7 +8991,7 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>Mycobacterium houstonense</t>
+          <t>Mycobacterium fluoranthenivorans</t>
         </is>
       </c>
     </row>
@@ -9007,7 +9003,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>B_MYCBC_IMMN</t>
+          <t>B_MYCBC_FRTT</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
@@ -9017,7 +9013,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>Mycobacterium immunogenum</t>
+          <t>Mycobacterium fortuitum</t>
         </is>
       </c>
     </row>
@@ -9029,7 +9025,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>B_MYCBC_INSB</t>
+          <t>B_MYCBC_FRTT_ACTM</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
@@ -9039,7 +9035,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>Mycobacterium insubricum</t>
+          <t>Mycobacterium fortuitum acetamidolyticum</t>
         </is>
       </c>
     </row>
@@ -9051,7 +9047,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>B_MYCBC_IRNC</t>
+          <t>B_MYCBC_FRTT_FRTT</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
@@ -9061,7 +9057,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>Mycobacterium iranicum</t>
+          <t>Mycobacterium fortuitum fortuitum</t>
         </is>
       </c>
     </row>
@@ -9073,7 +9069,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>B_MYCBC_KMSS</t>
+          <t>B_MYCBC_FRNK</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
@@ -9083,7 +9079,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>Mycobacterium komossense</t>
+          <t>Mycobacterium franklinii</t>
         </is>
       </c>
     </row>
@@ -9095,7 +9091,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>B_MYCBC_LTRL</t>
+          <t>B_MYCBC_FRDR</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
@@ -9105,7 +9101,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>Mycobacterium litorale</t>
+          <t>Mycobacterium frederiksbergense</t>
         </is>
       </c>
     </row>
@@ -9117,7 +9113,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>B_MYCBC_LLTZ</t>
+          <t>B_MYCBC_GADM</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
@@ -9127,7 +9123,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>Mycobacterium llatzerense</t>
+          <t>Mycobacterium gadium</t>
         </is>
       </c>
     </row>
@@ -9139,7 +9135,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>B_MYCBC_MDGS</t>
+          <t>B_MYCBC_GLVM</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
@@ -9149,7 +9145,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>Mycobacterium madagascariense</t>
+          <t>Mycobacterium gilvum</t>
         </is>
       </c>
     </row>
@@ -9161,7 +9157,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>B_MYCBC_MGRT</t>
+          <t>B_MYCBC_GOOD</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
@@ -9171,7 +9167,7 @@
       </c>
       <c r="D400" t="inlineStr">
         <is>
-          <t>Mycobacterium mageritense</t>
+          <t>Mycobacterium goodii</t>
         </is>
       </c>
     </row>
@@ -9183,7 +9179,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>B_MYCBC_MNCN</t>
+          <t>B_MYCBC_HSSC</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
@@ -9193,7 +9189,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>Mycobacterium monacense</t>
+          <t>Mycobacterium hassiacum</t>
         </is>
       </c>
     </row>
@@ -9205,7 +9201,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>B_MYCBC_MRKN</t>
+          <t>B_MYCBC_HPPC</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
@@ -9215,7 +9211,7 @@
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>Mycobacterium moriokaense</t>
+          <t>Mycobacterium hippocampi</t>
         </is>
       </c>
     </row>
@@ -9227,7 +9223,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>B_MYCBC_MCGN</t>
+          <t>B_MYCBC_HDLR</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
@@ -9237,7 +9233,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>Mycobacterium mucogenicum</t>
+          <t>Mycobacterium hodleri</t>
         </is>
       </c>
     </row>
@@ -9249,7 +9245,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>B_MYCBC_MURL</t>
+          <t>B_MYCBC_HLST</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
@@ -9259,7 +9255,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>Mycobacterium murale</t>
+          <t>Mycobacterium holsaticum</t>
         </is>
       </c>
     </row>
@@ -9271,7 +9267,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>B_MYCBC_NERM</t>
+          <t>B_MYCBC_HSTN</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
@@ -9281,7 +9277,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>Mycobacterium neoaurum</t>
+          <t>Mycobacterium houstonense</t>
         </is>
       </c>
     </row>
@@ -9293,7 +9289,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>B_MYCBC_NWRL</t>
+          <t>B_MYCBC_IMMN</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
@@ -9303,7 +9299,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>Mycobacterium neworleansense</t>
+          <t>Mycobacterium immunogenum</t>
         </is>
       </c>
     </row>
@@ -9315,7 +9311,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>B_MYCBC_NVCS</t>
+          <t>B_MYCBC_INSB</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
@@ -9325,7 +9321,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>Mycobacterium novocastrense</t>
+          <t>Mycobacterium insubricum</t>
         </is>
       </c>
     </row>
@@ -9337,7 +9333,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>B_MYCBC_OBNS</t>
+          <t>B_MYCBC_IRNC</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
@@ -9347,7 +9343,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>Mycobacterium obuense</t>
+          <t>Mycobacterium iranicum</t>
         </is>
       </c>
     </row>
@@ -9359,7 +9355,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>B_MYCBC_PLLN</t>
+          <t>B_MYCBC_KMSS</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
@@ -9369,7 +9365,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>Mycobacterium pallens</t>
+          <t>Mycobacterium komossense</t>
         </is>
       </c>
     </row>
@@ -9381,7 +9377,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>B_MYCBC_PRFR</t>
+          <t>B_MYCBC_LTRL</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
@@ -9391,7 +9387,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>Mycobacterium parafortuitum</t>
+          <t>Mycobacterium litorale</t>
         </is>
       </c>
     </row>
@@ -9403,7 +9399,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>B_MYCBC_GRNM</t>
+          <t>B_MYCBC_LLTZ</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
@@ -9413,7 +9409,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>Mycobacterium peregrinum</t>
+          <t>Mycobacterium llatzerense</t>
         </is>
       </c>
     </row>
@@ -9425,7 +9421,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>B_MYCBC_PHLE</t>
+          <t>B_MYCBC_MDGS</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
@@ -9435,7 +9431,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>Mycobacterium phlei</t>
+          <t>Mycobacterium madagascariense</t>
         </is>
       </c>
     </row>
@@ -9447,7 +9443,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>B_MYCBC_PHCC</t>
+          <t>B_MYCBC_MGRT</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
@@ -9457,7 +9453,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>Mycobacterium phocaicum</t>
+          <t>Mycobacterium mageritense</t>
         </is>
       </c>
     </row>
@@ -9469,7 +9465,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>B_MYCBC_PRCN</t>
+          <t>B_MYCBC_MNCN</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
@@ -9479,7 +9475,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>Mycobacterium porcinum</t>
+          <t>Mycobacterium monacense</t>
         </is>
       </c>
     </row>
@@ -9491,7 +9487,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>B_MYCBC_RFRE</t>
+          <t>B_MYCBC_MRKN</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
@@ -9501,7 +9497,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>Mycobacterium poriferae</t>
+          <t>Mycobacterium moriokaense</t>
         </is>
       </c>
     </row>
@@ -9513,7 +9509,7 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>B_MYCBC_PSYC</t>
+          <t>B_MYCBC_MCGN</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
@@ -9523,7 +9519,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>Mycobacterium psychrotolerans</t>
+          <t>Mycobacterium mucogenicum</t>
         </is>
       </c>
     </row>
@@ -9535,7 +9531,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>B_MYCBC_PYRN</t>
+          <t>B_MYCBC_MURL</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
@@ -9545,7 +9541,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>Mycobacterium pyrenivorans</t>
+          <t>Mycobacterium murale</t>
         </is>
       </c>
     </row>
@@ -9557,7 +9553,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>B_MYCBC_RHDS</t>
+          <t>B_MYCBC_NERM</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
@@ -9567,7 +9563,7 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>Mycobacterium rhodesiae</t>
+          <t>Mycobacterium neoaurum</t>
         </is>
       </c>
     </row>
@@ -9579,7 +9575,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>B_MYCBC_RUFM</t>
+          <t>B_MYCBC_NWRL</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
@@ -9589,7 +9585,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>Mycobacterium rufum</t>
+          <t>Mycobacterium neworleansense</t>
         </is>
       </c>
     </row>
@@ -9601,7 +9597,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>B_MYCBC_RTLM</t>
+          <t>B_MYCBC_NVCS</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
@@ -9611,7 +9607,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>Mycobacterium rutilum</t>
+          <t>Mycobacterium novocastrense</t>
         </is>
       </c>
     </row>
@@ -9623,7 +9619,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>B_MYCBC_SLMN</t>
+          <t>B_MYCBC_OBNS</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
@@ -9633,7 +9629,7 @@
       </c>
       <c r="D421" t="inlineStr">
         <is>
-          <t>Mycobacterium salmoniphilum</t>
+          <t>Mycobacterium obuense</t>
         </is>
       </c>
     </row>
@@ -9645,7 +9641,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>B_MYCBC_SDMN</t>
+          <t>B_MYCBC_PLLN</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
@@ -9655,7 +9651,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>Mycobacterium sediminis</t>
+          <t>Mycobacterium pallens</t>
         </is>
       </c>
     </row>
@@ -9667,7 +9663,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>B_MYCBC_SNGL</t>
+          <t>B_MYCBC_PRFR</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
@@ -9677,7 +9673,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>Mycobacterium senegalense</t>
+          <t>Mycobacterium parafortuitum</t>
         </is>
       </c>
     </row>
@@ -9689,7 +9685,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>B_MYCBC_SPTC</t>
+          <t>B_MYCBC_GRNM</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
@@ -9699,7 +9695,7 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>Mycobacterium septicum</t>
+          <t>Mycobacterium peregrinum</t>
         </is>
       </c>
     </row>
@@ -9711,7 +9707,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>B_MYCBC_STNS</t>
+          <t>B_MYCBC_PHLE</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
@@ -9721,7 +9717,7 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>Mycobacterium setense</t>
+          <t>Mycobacterium phlei</t>
         </is>
       </c>
     </row>
@@ -9733,7 +9729,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>B_MYCBC_SMGM</t>
+          <t>B_MYCBC_PHCC</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
@@ -9743,7 +9739,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>Mycobacterium smegmatis</t>
+          <t>Mycobacterium phocaicum</t>
         </is>
       </c>
     </row>
@@ -9755,7 +9751,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>B_MYCBC_SPHG</t>
+          <t>B_MYCBC_PRCN</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
@@ -9765,7 +9761,7 @@
       </c>
       <c r="D427" t="inlineStr">
         <is>
-          <t>Mycobacterium sphagni</t>
+          <t>Mycobacterium porcinum</t>
         </is>
       </c>
     </row>
@@ -9777,7 +9773,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>B_MYCBC_THRM</t>
+          <t>B_MYCBC_RFRE</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
@@ -9787,7 +9783,7 @@
       </c>
       <c r="D428" t="inlineStr">
         <is>
-          <t>Mycobacterium thermoresistibile</t>
+          <t>Mycobacterium poriferae</t>
         </is>
       </c>
     </row>
@@ -9799,7 +9795,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>B_MYCBC_TKNS</t>
+          <t>B_MYCBC_PSYC</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
@@ -9809,7 +9805,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>Mycobacterium tokaiense</t>
+          <t>Mycobacterium psychrotolerans</t>
         </is>
       </c>
     </row>
@@ -9821,7 +9817,7 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>B_MYCBC_VACC</t>
+          <t>B_MYCBC_PYRN</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
@@ -9831,7 +9827,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>Mycobacterium vaccae</t>
+          <t>Mycobacterium pyrenivorans</t>
         </is>
       </c>
     </row>
@@ -9843,7 +9839,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>B_MYCBC_ASTR</t>
+          <t>B_MYCBC_RHDS</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
@@ -9853,7 +9849,7 @@
       </c>
       <c r="D431" t="inlineStr">
         <is>
-          <t>Mycobacterium vanbaalenii</t>
+          <t>Mycobacterium rhodesiae</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9861,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>B_MYCBC_WLNS</t>
+          <t>B_MYCBC_RUFM</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
@@ -9875,513 +9871,513 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>Mycobacterium wolinskyi</t>
+          <t>Mycobacterium rufum</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>B_MYCBC_FRCN</t>
+          <t>B_MYCBC_RTLM</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D433" t="inlineStr">
         <is>
-          <t>Mycobacterium farcinogenes</t>
+          <t>Mycobacterium rutilum</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>B_MYCBC_GSTR</t>
+          <t>B_MYCBC_SLMN</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>Mycobacterium gastri</t>
+          <t>Mycobacterium salmoniphilum</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>B_MYCBC_GNVN</t>
+          <t>B_MYCBC_SDMN</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>Mycobacterium genavense</t>
+          <t>Mycobacterium sediminis</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>B_MYCBC_HMPH</t>
+          <t>B_MYCBC_SNGL</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>Mycobacterium haemophilum</t>
+          <t>Mycobacterium senegalense</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>B_MYCBC_KNSS</t>
+          <t>B_MYCBC_SPTC</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D437" t="inlineStr">
         <is>
-          <t>Mycobacterium kansasii</t>
+          <t>Mycobacterium septicum</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>B_MYCBC_LEPR</t>
+          <t>B_MYCBC_STNS</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>Mycobacterium leprae</t>
+          <t>Mycobacterium setense</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>B_MYCBC_LPRM</t>
+          <t>B_MYCBC_SMGM</t>
         </is>
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>Mycobacterium lepraemurium</t>
+          <t>Mycobacterium smegmatis</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>B_MYCBC_MLMN</t>
+          <t>B_MYCBC_SPHG</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D440" t="inlineStr">
         <is>
-          <t>Mycobacterium malmoense</t>
+          <t>Mycobacterium sphagni</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>B_MYCBC_SGM</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>B_MYCBC_MRNM</t>
+          <t>B_MYCBC_THRM</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>Slowly growing Mycobacterium (SGM)</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>Mycobacterium marinum</t>
+          <t>Mycobacterium thermoresistibile</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPA</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>B_STRPT_PYGN</t>
+          <t>B_MYCBC_TKNS</t>
         </is>
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>Streptococcus Group A</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D442" t="inlineStr">
         <is>
-          <t>Streptococcus pyogenes</t>
+          <t>Mycobacterium tokaiense</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPA</t>
+          <t>B_MYCBC_VACC</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>Streptococcus Group A</t>
+          <t>Mycobacterium vaccae</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPB</t>
+          <t>B_MYCBC_ASTR</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>Streptococcus Group B</t>
+          <t>Mycobacterium vanbaalenii</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_RGM</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPC</t>
+          <t>B_MYCBC_WLNS</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Rapidly growing Mycobacterium (RGM)</t>
         </is>
       </c>
       <c r="D445" t="inlineStr">
         <is>
-          <t>Streptococcus Group C</t>
+          <t>Mycobacterium wolinskyi</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPG</t>
+          <t>B_MYCBC_FRCN</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D446" t="inlineStr">
         <is>
-          <t>Streptococcus Group G</t>
+          <t>Mycobacterium farcinogenes</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>B_STRPT_AGLC</t>
+          <t>B_MYCBC_GSTR</t>
         </is>
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D447" t="inlineStr">
         <is>
-          <t>Streptococcus agalactiae</t>
+          <t>Mycobacterium gastri</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>B_STRPT_CANS</t>
+          <t>B_MYCBC_GNVN</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>Streptococcus canis</t>
+          <t>Mycobacterium genavense</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG</t>
+          <t>B_MYCBC_HMPH</t>
         </is>
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D449" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae</t>
+          <t>Mycobacterium haemophilum</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG_DYSG</t>
+          <t>B_MYCBC_KNSS</t>
         </is>
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D450" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae dysgalactiae</t>
+          <t>Mycobacterium kansasii</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG_EQSM</t>
+          <t>B_MYCBC_LEPR</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D451" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae equisimilis</t>
+          <t>Mycobacterium leprae</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>B_STRPT_EQUI</t>
+          <t>B_MYCBC_LPRM</t>
         </is>
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D452" t="inlineStr">
         <is>
-          <t>Streptococcus equi</t>
+          <t>Mycobacterium lepraemurium</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>B_STRPT_EQUI_EQUI</t>
+          <t>B_MYCBC_MLMN</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>Streptococcus equi equi</t>
+          <t>Mycobacterium malmoense</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_MYCBC_SGM</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>B_STRPT_EQUI_RMNT</t>
+          <t>B_MYCBC_MRNM</t>
         </is>
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Slowly growing Mycobacterium (SGM)</t>
         </is>
       </c>
       <c r="D454" t="inlineStr">
         <is>
-          <t>Streptococcus equi ruminatorum</t>
+          <t>Mycobacterium marinum</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>B_STRPT_ABCG</t>
+          <t>B_STRPT_GRPA</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>B_STRPT_EQUI_ZPDM</t>
+          <t>B_STRPT_PYGN</t>
         </is>
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>Streptococcus Group A, B, C, G</t>
+          <t>Streptococcus Group A</t>
         </is>
       </c>
       <c r="D455" t="inlineStr">
         <is>
-          <t>Streptococcus equi zooepidemicus</t>
+          <t>Streptococcus pyogenes</t>
         </is>
       </c>
     </row>
@@ -10393,7 +10389,7 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>B_STRPT_PYGN</t>
+          <t>B_STRPT_GRPA</t>
         </is>
       </c>
       <c r="C456" t="inlineStr">
@@ -10403,887 +10399,887 @@
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>Streptococcus pyogenes</t>
+          <t>Streptococcus Group A</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
+          <t>B_STRPT_ABCG</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
           <t>B_STRPT_GRPB</t>
         </is>
       </c>
-      <c r="B457" t="inlineStr">
-        <is>
-          <t>B_STRPT_AGLC</t>
-        </is>
-      </c>
       <c r="C457" t="inlineStr">
         <is>
+          <t>Streptococcus Group A, B, C, G</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
           <t>Streptococcus Group B</t>
-        </is>
-      </c>
-      <c r="D457" t="inlineStr">
-        <is>
-          <t>Streptococcus agalactiae</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
+          <t>B_STRPT_ABCG</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
           <t>B_STRPT_GRPC</t>
         </is>
       </c>
-      <c r="B458" t="inlineStr">
-        <is>
-          <t>B_STRPT_DYSG</t>
-        </is>
-      </c>
       <c r="C458" t="inlineStr">
         <is>
+          <t>Streptococcus Group A, B, C, G</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
           <t>Streptococcus Group C</t>
-        </is>
-      </c>
-      <c r="D458" t="inlineStr">
-        <is>
-          <t>Streptococcus dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPC</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG_DYSG</t>
+          <t>B_STRPT_GRPG</t>
         </is>
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>Streptococcus Group C</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae dysgalactiae</t>
+          <t>Streptococcus Group G</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPC</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG_EQSM</t>
+          <t>B_STRPT_AGLC</t>
         </is>
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>Streptococcus Group C</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D460" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae equisimilis</t>
+          <t>Streptococcus agalactiae</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPC</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>B_STRPT_EQUI</t>
+          <t>B_STRPT_CANS</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>Streptococcus Group C</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D461" t="inlineStr">
         <is>
-          <t>Streptococcus equi</t>
+          <t>Streptococcus canis</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPC</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>B_STRPT_EQUI_EQUI</t>
+          <t>B_STRPT_DYSG</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>Streptococcus Group C</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D462" t="inlineStr">
         <is>
-          <t>Streptococcus equi equi</t>
+          <t>Streptococcus dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPC</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>B_STRPT_EQUI_RMNT</t>
+          <t>B_STRPT_DYSG_DYSG</t>
         </is>
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>Streptococcus Group C</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D463" t="inlineStr">
         <is>
-          <t>Streptococcus equi ruminatorum</t>
+          <t>Streptococcus dysgalactiae dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPC</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>B_STRPT_EQUI_ZPDM</t>
+          <t>B_STRPT_DYSG_EQSM</t>
         </is>
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>Streptococcus Group C</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>Streptococcus equi zooepidemicus</t>
+          <t>Streptococcus dysgalactiae equisimilis</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPF</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>B_STRPT_ANGN</t>
+          <t>B_STRPT_EQUI</t>
         </is>
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>Streptococcus Group F</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>Streptococcus anginosus</t>
+          <t>Streptococcus equi</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPF</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>B_STRPT_ANGN_ANGN</t>
+          <t>B_STRPT_EQUI_EQUI</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>Streptococcus Group F</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>Streptococcus anginosus anginosus</t>
+          <t>Streptococcus equi equi</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPF</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>B_STRPT_ANGN_WHLY</t>
+          <t>B_STRPT_EQUI_RMNT</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>Streptococcus Group F</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>Streptococcus anginosus whileyi</t>
+          <t>Streptococcus equi ruminatorum</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPF</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>B_STRPT_CNST</t>
+          <t>B_STRPT_EQUI_ZPDM</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>Streptococcus Group F</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>Streptococcus constellatus</t>
+          <t>Streptococcus equi zooepidemicus</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPF</t>
+          <t>B_STRPT_ABCG</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>B_STRPT_CNST_CNST</t>
+          <t>B_STRPT_PYGN</t>
         </is>
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>Streptococcus Group F</t>
+          <t>Streptococcus Group A, B, C, G</t>
         </is>
       </c>
       <c r="D469" t="inlineStr">
         <is>
-          <t>Streptococcus constellatus constellatus</t>
+          <t>Streptococcus pyogenes</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPF</t>
+          <t>B_STRPT_GRPB</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>B_STRPT_CNST_PHRY</t>
+          <t>B_STRPT_AGLC</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>Streptococcus Group F</t>
+          <t>Streptococcus Group B</t>
         </is>
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>Streptococcus constellatus pharyngis</t>
+          <t>Streptococcus agalactiae</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPF</t>
+          <t>B_STRPT_GRPC</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>B_STRPT_CNST_VBRG</t>
+          <t>B_STRPT_DYSG</t>
         </is>
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>Streptococcus Group F</t>
+          <t>Streptococcus Group C</t>
         </is>
       </c>
       <c r="D471" t="inlineStr">
         <is>
-          <t>Streptococcus constellatus viborgensis</t>
+          <t>Streptococcus dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPF</t>
+          <t>B_STRPT_GRPC</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>B_STRPT_INTR</t>
+          <t>B_STRPT_DYSG_DYSG</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>Streptococcus Group F</t>
+          <t>Streptococcus Group C</t>
         </is>
       </c>
       <c r="D472" t="inlineStr">
         <is>
-          <t>Streptococcus intermedius</t>
+          <t>Streptococcus dysgalactiae dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPG</t>
+          <t>B_STRPT_GRPC</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>B_STRPT_CANS</t>
+          <t>B_STRPT_DYSG_EQSM</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>Streptococcus Group G</t>
+          <t>Streptococcus Group C</t>
         </is>
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>Streptococcus canis</t>
+          <t>Streptococcus dysgalactiae equisimilis</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPG</t>
+          <t>B_STRPT_GRPC</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG</t>
+          <t>B_STRPT_EQUI</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>Streptococcus Group G</t>
+          <t>Streptococcus Group C</t>
         </is>
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae</t>
+          <t>Streptococcus equi</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPG</t>
+          <t>B_STRPT_GRPC</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG_DYSG</t>
+          <t>B_STRPT_EQUI_EQUI</t>
         </is>
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>Streptococcus Group G</t>
+          <t>Streptococcus Group C</t>
         </is>
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae dysgalactiae</t>
+          <t>Streptococcus equi equi</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPG</t>
+          <t>B_STRPT_GRPC</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG_EQSM</t>
+          <t>B_STRPT_EQUI_RMNT</t>
         </is>
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>Streptococcus Group G</t>
+          <t>Streptococcus Group C</t>
         </is>
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae equisimilis</t>
+          <t>Streptococcus equi ruminatorum</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPH</t>
+          <t>B_STRPT_GRPC</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>B_STRPT_SNGN</t>
+          <t>B_STRPT_EQUI_ZPDM</t>
         </is>
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>Streptococcus Group H</t>
+          <t>Streptococcus Group C</t>
         </is>
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>Streptococcus sanguinis</t>
+          <t>Streptococcus equi zooepidemicus</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPK</t>
+          <t>B_STRPT_GRPF</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>B_STRPT_SLVR</t>
+          <t>B_STRPT_ANGN</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>Streptococcus Group K</t>
+          <t>Streptococcus Group F</t>
         </is>
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>Streptococcus salivarius</t>
+          <t>Streptococcus anginosus</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPK</t>
+          <t>B_STRPT_GRPF</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>B_STRPT_SLVR</t>
+          <t>B_STRPT_ANGN_ANGN</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>Streptococcus Group K</t>
+          <t>Streptococcus Group F</t>
         </is>
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>Streptococcus salivarius salivarius</t>
+          <t>Streptococcus anginosus anginosus</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPK</t>
+          <t>B_STRPT_GRPF</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>B_STRPT_THRM</t>
+          <t>B_STRPT_ANGN_WHLY</t>
         </is>
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>Streptococcus Group K</t>
+          <t>Streptococcus Group F</t>
         </is>
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>Streptococcus salivarius thermophilus</t>
+          <t>Streptococcus anginosus whileyi</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPL</t>
+          <t>B_STRPT_GRPF</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG</t>
+          <t>B_STRPT_CNST</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>Streptococcus Group L</t>
+          <t>Streptococcus Group F</t>
         </is>
       </c>
       <c r="D481" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae</t>
+          <t>Streptococcus constellatus</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPL</t>
+          <t>B_STRPT_GRPF</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG_DYSG</t>
+          <t>B_STRPT_CNST_CNST</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>Streptococcus Group L</t>
+          <t>Streptococcus Group F</t>
         </is>
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae dysgalactiae</t>
+          <t>Streptococcus constellatus constellatus</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>B_STRPT_GRPL</t>
+          <t>B_STRPT_GRPF</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>B_STRPT_DYSG_EQSM</t>
+          <t>B_STRPT_CNST_PHRY</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>Streptococcus Group L</t>
+          <t>Streptococcus Group F</t>
         </is>
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>Streptococcus dysgalactiae equisimilis</t>
+          <t>Streptococcus constellatus pharyngis</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPF</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>B_STRPT_MILL</t>
+          <t>B_STRPT_CNST_VBRG</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group F</t>
         </is>
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>Milleri Group Streptococcus (MGS)</t>
+          <t>Streptococcus constellatus viborgensis</t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPF</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>B_STRPT_ACDM</t>
+          <t>B_STRPT_INTR</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group F</t>
         </is>
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>Streptococcus acidominimus</t>
+          <t>Streptococcus intermedius</t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPG</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>B_STRPT_ANGN</t>
+          <t>B_STRPT_CANS</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group G</t>
         </is>
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>Streptococcus anginosus</t>
+          <t>Streptococcus canis</t>
         </is>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPG</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>B_STRPT_ANGN_ANGN</t>
+          <t>B_STRPT_DYSG</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group G</t>
         </is>
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>Streptococcus anginosus anginosus</t>
+          <t>Streptococcus dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPG</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>B_STRPT_ANGN_WHLY</t>
+          <t>B_STRPT_DYSG_DYSG</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group G</t>
         </is>
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>Streptococcus anginosus whileyi</t>
+          <t>Streptococcus dysgalactiae dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPG</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>B_STRPT_CNST</t>
+          <t>B_STRPT_DYSG_EQSM</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group G</t>
         </is>
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>Streptococcus constellatus</t>
+          <t>Streptococcus dysgalactiae equisimilis</t>
         </is>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPH</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>B_STRPT_CNST_CNST</t>
+          <t>B_STRPT_SNGN</t>
         </is>
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group H</t>
         </is>
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>Streptococcus constellatus constellatus</t>
+          <t>Streptococcus sanguinis</t>
         </is>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPK</t>
         </is>
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>B_STRPT_CNST_PHRY</t>
+          <t>B_STRPT_SLVR</t>
         </is>
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group K</t>
         </is>
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>Streptococcus constellatus pharyngis</t>
+          <t>Streptococcus salivarius</t>
         </is>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPK</t>
         </is>
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>B_STRPT_CNST_VBRG</t>
+          <t>B_STRPT_SLVR</t>
         </is>
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group K</t>
         </is>
       </c>
       <c r="D492" t="inlineStr">
         <is>
-          <t>Streptococcus constellatus viborgensis</t>
+          <t>Streptococcus salivarius salivarius</t>
         </is>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPK</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>B_STRPT_CRCT</t>
+          <t>B_STRPT_THRM</t>
         </is>
       </c>
       <c r="C493" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group K</t>
         </is>
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>Streptococcus criceti</t>
+          <t>Streptococcus salivarius thermophilus</t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPL</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>B_STRPT_CRST</t>
+          <t>B_STRPT_DYSG</t>
         </is>
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group L</t>
         </is>
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>Streptococcus cristatus</t>
+          <t>Streptococcus dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPL</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>B_STRPT_DOWN</t>
+          <t>B_STRPT_DYSG_DYSG</t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group L</t>
         </is>
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>Streptococcus downei</t>
+          <t>Streptococcus dysgalactiae dysgalactiae</t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>B_STRPT_VIRI</t>
+          <t>B_STRPT_GRPL</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>B_STRPT_EQNS</t>
+          <t>B_STRPT_DYSG_EQSM</t>
         </is>
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>Viridans Group Streptococcus (VGS)</t>
+          <t>Streptococcus Group L</t>
         </is>
       </c>
       <c r="D496" t="inlineStr">
         <is>
-          <t>Streptococcus equinus</t>
+          <t>Streptococcus dysgalactiae equisimilis</t>
         </is>
       </c>
     </row>
@@ -11295,7 +11291,7 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>B_STRPT_FERS</t>
+          <t>B_STRPT_MILL</t>
         </is>
       </c>
       <c r="C497" t="inlineStr">
@@ -11305,7 +11301,7 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>Streptococcus ferus</t>
+          <t>Milleri Group Streptococcus (MGS)</t>
         </is>
       </c>
     </row>
@@ -11317,7 +11313,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>B_STRPT_GRDN</t>
+          <t>B_STRPT_ACDM</t>
         </is>
       </c>
       <c r="C498" t="inlineStr">
@@ -11327,7 +11323,7 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>Streptococcus gordonii</t>
+          <t>Streptococcus acidominimus</t>
         </is>
       </c>
     </row>
@@ -11339,7 +11335,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>B_STRPT_INTR</t>
+          <t>B_STRPT_ANGN</t>
         </is>
       </c>
       <c r="C499" t="inlineStr">
@@ -11349,7 +11345,7 @@
       </c>
       <c r="D499" t="inlineStr">
         <is>
-          <t>Streptococcus intermedius</t>
+          <t>Streptococcus anginosus</t>
         </is>
       </c>
     </row>
@@ -11361,7 +11357,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>B_STRPT_MACC</t>
+          <t>B_STRPT_ANGN_ANGN</t>
         </is>
       </c>
       <c r="C500" t="inlineStr">
@@ -11371,7 +11367,7 @@
       </c>
       <c r="D500" t="inlineStr">
         <is>
-          <t>Streptococcus macacae</t>
+          <t>Streptococcus anginosus anginosus</t>
         </is>
       </c>
     </row>
@@ -11383,7 +11379,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>B_STRPT_MITS</t>
+          <t>B_STRPT_ANGN_WHLY</t>
         </is>
       </c>
       <c r="C501" t="inlineStr">
@@ -11393,7 +11389,7 @@
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>Streptococcus mitis</t>
+          <t>Streptococcus anginosus whileyi</t>
         </is>
       </c>
     </row>
@@ -11405,7 +11401,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>B_STRPT_MTNS</t>
+          <t>B_STRPT_CNST</t>
         </is>
       </c>
       <c r="C502" t="inlineStr">
@@ -11415,7 +11411,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>Streptococcus mutans</t>
+          <t>Streptococcus constellatus</t>
         </is>
       </c>
     </row>
@@ -11427,7 +11423,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>B_STRPT_ORLS</t>
+          <t>B_STRPT_CNST_CNST</t>
         </is>
       </c>
       <c r="C503" t="inlineStr">
@@ -11437,7 +11433,7 @@
       </c>
       <c r="D503" t="inlineStr">
         <is>
-          <t>Streptococcus oralis</t>
+          <t>Streptococcus constellatus constellatus</t>
         </is>
       </c>
     </row>
@@ -11449,7 +11445,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>B_STRPT_ORLS_DNTS</t>
+          <t>B_STRPT_CNST_PHRY</t>
         </is>
       </c>
       <c r="C504" t="inlineStr">
@@ -11459,7 +11455,7 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>Streptococcus oralis dentisani</t>
+          <t>Streptococcus constellatus pharyngis</t>
         </is>
       </c>
     </row>
@@ -11471,7 +11467,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>B_STRPT_ORLS_ORLS</t>
+          <t>B_STRPT_CNST_VBRG</t>
         </is>
       </c>
       <c r="C505" t="inlineStr">
@@ -11481,7 +11477,7 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>Streptococcus oralis oralis</t>
+          <t>Streptococcus constellatus viborgensis</t>
         </is>
       </c>
     </row>
@@ -11493,7 +11489,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>B_STRPT_ORLS_TGRN</t>
+          <t>B_STRPT_CRCT</t>
         </is>
       </c>
       <c r="C506" t="inlineStr">
@@ -11503,7 +11499,7 @@
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>Streptococcus oralis tigurinus</t>
+          <t>Streptococcus criceti</t>
         </is>
       </c>
     </row>
@@ -11515,7 +11511,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>B_STRPT_PRSN</t>
+          <t>B_STRPT_CRST</t>
         </is>
       </c>
       <c r="C507" t="inlineStr">
@@ -11525,7 +11521,7 @@
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>Streptococcus parasanguinis</t>
+          <t>Streptococcus cristatus</t>
         </is>
       </c>
     </row>
@@ -11537,7 +11533,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>B_STRPT_RATT</t>
+          <t>B_STRPT_DOWN</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
@@ -11547,7 +11543,7 @@
       </c>
       <c r="D508" t="inlineStr">
         <is>
-          <t>Streptococcus ratti</t>
+          <t>Streptococcus downei</t>
         </is>
       </c>
     </row>
@@ -11559,7 +11555,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>B_STRPT_SLVR</t>
+          <t>B_STRPT_EQNS</t>
         </is>
       </c>
       <c r="C509" t="inlineStr">
@@ -11569,7 +11565,7 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>Streptococcus salivarius</t>
+          <t>Streptococcus equinus</t>
         </is>
       </c>
     </row>
@@ -11581,7 +11577,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>B_STRPT_SLVR</t>
+          <t>B_STRPT_FERS</t>
         </is>
       </c>
       <c r="C510" t="inlineStr">
@@ -11591,7 +11587,7 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>Streptococcus salivarius salivarius</t>
+          <t>Streptococcus ferus</t>
         </is>
       </c>
     </row>
@@ -11603,7 +11599,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>B_STRPT_THRM</t>
+          <t>B_STRPT_GRDN</t>
         </is>
       </c>
       <c r="C511" t="inlineStr">
@@ -11613,7 +11609,7 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>Streptococcus salivarius thermophilus</t>
+          <t>Streptococcus gordonii</t>
         </is>
       </c>
     </row>
@@ -11625,7 +11621,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>B_STRPT_SNGN</t>
+          <t>B_STRPT_INTR</t>
         </is>
       </c>
       <c r="C512" t="inlineStr">
@@ -11635,7 +11631,7 @@
       </c>
       <c r="D512" t="inlineStr">
         <is>
-          <t>Streptococcus sanguinis</t>
+          <t>Streptococcus intermedius</t>
         </is>
       </c>
     </row>
@@ -11647,7 +11643,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>B_STRPT_SBRN</t>
+          <t>B_STRPT_MACC</t>
         </is>
       </c>
       <c r="C513" t="inlineStr">
@@ -11657,7 +11653,7 @@
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>Streptococcus sobrinus</t>
+          <t>Streptococcus macacae</t>
         </is>
       </c>
     </row>
@@ -11669,7 +11665,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>B_STRPT_SUIS</t>
+          <t>B_STRPT_MITS</t>
         </is>
       </c>
       <c r="C514" t="inlineStr">
@@ -11679,7 +11675,7 @@
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>Streptococcus suis</t>
+          <t>Streptococcus mitis</t>
         </is>
       </c>
     </row>
@@ -11691,7 +11687,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>B_STRPT_UBRS</t>
+          <t>B_STRPT_MTNS</t>
         </is>
       </c>
       <c r="C515" t="inlineStr">
@@ -11701,7 +11697,7 @@
       </c>
       <c r="D515" t="inlineStr">
         <is>
-          <t>Streptococcus uberis</t>
+          <t>Streptococcus mutans</t>
         </is>
       </c>
     </row>
@@ -11713,7 +11709,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>B_STRPT_VSTB</t>
+          <t>B_STRPT_ORLS</t>
         </is>
       </c>
       <c r="C516" t="inlineStr">
@@ -11723,137 +11719,423 @@
       </c>
       <c r="D516" t="inlineStr">
         <is>
-          <t>Streptococcus vestibularis</t>
+          <t>Streptococcus oralis</t>
         </is>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>B_YERSN_PSDT-C</t>
+          <t>B_STRPT_VIRI</t>
         </is>
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>B_YERSN_PSTS</t>
+          <t>B_STRPT_ORLS_DNTS</t>
         </is>
       </c>
       <c r="C517" t="inlineStr">
         <is>
-          <t>Yersinia pseudotuberculosis complex</t>
+          <t>Viridans Group Streptococcus (VGS)</t>
         </is>
       </c>
       <c r="D517" t="inlineStr">
         <is>
-          <t>Yersinia pestis</t>
+          <t>Streptococcus oralis dentisani</t>
         </is>
       </c>
     </row>
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>B_YERSN_PSDT-C</t>
+          <t>B_STRPT_VIRI</t>
         </is>
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>B_YERSN_PSDT</t>
+          <t>B_STRPT_ORLS_ORLS</t>
         </is>
       </c>
       <c r="C518" t="inlineStr">
         <is>
-          <t>Yersinia pseudotuberculosis complex</t>
+          <t>Viridans Group Streptococcus (VGS)</t>
         </is>
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>Yersinia pseudotuberculosis</t>
+          <t>Streptococcus oralis oralis</t>
         </is>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
-          <t>B_YERSN_PSDT-C</t>
+          <t>B_STRPT_VIRI</t>
         </is>
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>B_YERSN_PSTS</t>
+          <t>B_STRPT_ORLS_TGRN</t>
         </is>
       </c>
       <c r="C519" t="inlineStr">
         <is>
-          <t>Yersinia pseudotuberculosis complex</t>
+          <t>Viridans Group Streptococcus (VGS)</t>
         </is>
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>Yersinia pseudotuberculosis pestis</t>
+          <t>Streptococcus oralis tigurinus</t>
         </is>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="inlineStr">
         <is>
-          <t>B_YERSN_PSDT-C</t>
+          <t>B_STRPT_VIRI</t>
         </is>
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>B_YERSN_PSDT</t>
+          <t>B_STRPT_PRSN</t>
         </is>
       </c>
       <c r="C520" t="inlineStr">
         <is>
-          <t>Yersinia pseudotuberculosis complex</t>
+          <t>Viridans Group Streptococcus (VGS)</t>
         </is>
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>Yersinia pseudotuberculosis pseudotuberculosis</t>
+          <t>Streptococcus parasanguinis</t>
         </is>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="inlineStr">
         <is>
-          <t>B_YERSN_PSDT-C</t>
+          <t>B_STRPT_VIRI</t>
         </is>
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>B_YERSN_SMLS</t>
+          <t>B_STRPT_RATT</t>
         </is>
       </c>
       <c r="C521" t="inlineStr">
         <is>
-          <t>Yersinia pseudotuberculosis complex</t>
+          <t>Viridans Group Streptococcus (VGS)</t>
         </is>
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>Yersinia similis</t>
+          <t>Streptococcus ratti</t>
         </is>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
+          <t>B_STRPT_VIRI</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>B_STRPT_SLVR</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>Viridans Group Streptococcus (VGS)</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>Streptococcus salivarius</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>B_STRPT_VIRI</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>B_STRPT_SLVR</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>Viridans Group Streptococcus (VGS)</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>Streptococcus salivarius salivarius</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>B_STRPT_VIRI</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>B_STRPT_THRM</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>Viridans Group Streptococcus (VGS)</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>Streptococcus salivarius thermophilus</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>B_STRPT_VIRI</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>B_STRPT_SNGN</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>Viridans Group Streptococcus (VGS)</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>Streptococcus sanguinis</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>B_STRPT_VIRI</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>B_STRPT_SBRN</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>Viridans Group Streptococcus (VGS)</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>Streptococcus sobrinus</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>B_STRPT_VIRI</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>B_STRPT_SUIS</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>Viridans Group Streptococcus (VGS)</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>Streptococcus suis</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>B_STRPT_VIRI</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>B_STRPT_UBRS</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>Viridans Group Streptococcus (VGS)</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>Streptococcus uberis</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>B_STRPT_VIRI</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>B_STRPT_VSTB</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>Viridans Group Streptococcus (VGS)</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>Streptococcus vestibularis</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
           <t>B_YERSN_PSDT-C</t>
         </is>
       </c>
-      <c r="B522" t="inlineStr">
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSTS</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>Yersinia pseudotuberculosis complex</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>Yersinia pestis</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSDT-C</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSDT</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>Yersinia pseudotuberculosis complex</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>Yersinia pseudotuberculosis</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSDT-C</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSTS</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>Yersinia pseudotuberculosis complex</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>Yersinia pseudotuberculosis pestis</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSDT-C</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSDT</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>Yersinia pseudotuberculosis complex</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>Yersinia pseudotuberculosis pseudotuberculosis</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSDT-C</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>B_YERSN_SMLS</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>Yersinia pseudotuberculosis complex</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>Yersinia similis</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>B_YERSN_PSDT-C</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
         <is>
           <t>B_YERSN_WTRS</t>
         </is>
       </c>
-      <c r="C522" t="inlineStr">
+      <c r="C535" t="inlineStr">
         <is>
           <t>Yersinia pseudotuberculosis complex</t>
         </is>
       </c>
-      <c r="D522" t="inlineStr">
+      <c r="D535" t="inlineStr">
         <is>
           <t>Yersinia wautersii</t>
         </is>

</xml_diff>